<commit_message>
feat: Add new solution files for balanced and conservative scenarios, including exact and heuristic methods, and update experiment results with detailed resource allocation and performance metrics.
</commit_message>
<xml_diff>
--- a/results/solutions/experiment_results.xlsx
+++ b/results/solutions/experiment_results.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I4"/>
+  <dimension ref="A1:I7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -488,21 +488,23 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Heuristic</t>
+          <t>Exact</t>
         </is>
       </c>
       <c r="C2" t="n">
-        <v>734700</v>
+        <v>692450</v>
       </c>
       <c r="D2" t="n">
-        <v>7.002241134643555</v>
-      </c>
-      <c r="E2" t="inlineStr"/>
+        <v>1.320497274398804</v>
+      </c>
+      <c r="E2" t="n">
+        <v>0</v>
+      </c>
       <c r="F2" t="n">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="G2" t="n">
-        <v>212</v>
+        <v>207</v>
       </c>
       <c r="H2" t="n">
         <v>149</v>
@@ -512,7 +514,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Balanced</t>
+          <t>Conservative</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -521,51 +523,148 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>652185</v>
+        <v>734700</v>
       </c>
       <c r="D3" t="n">
-        <v>6.158377170562744</v>
-      </c>
-      <c r="E3" t="inlineStr"/>
+        <v>6.695088148117065</v>
+      </c>
+      <c r="E3" t="n">
+        <v>6.101523575709438</v>
+      </c>
       <c r="F3" t="n">
         <v>9</v>
       </c>
       <c r="G3" t="n">
-        <v>234</v>
+        <v>212</v>
       </c>
       <c r="H3" t="n">
-        <v>127</v>
+        <v>149</v>
       </c>
       <c r="I3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
+          <t>Balanced</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Exact</t>
+        </is>
+      </c>
+      <c r="C4" t="n">
+        <v>610175</v>
+      </c>
+      <c r="D4" t="n">
+        <v>0.2469408512115479</v>
+      </c>
+      <c r="E4" t="n">
+        <v>0</v>
+      </c>
+      <c r="F4" t="n">
+        <v>4</v>
+      </c>
+      <c r="G4" t="n">
+        <v>229</v>
+      </c>
+      <c r="H4" t="n">
+        <v>127</v>
+      </c>
+      <c r="I4" t="inlineStr"/>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Balanced</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Heuristic</t>
+        </is>
+      </c>
+      <c r="C5" t="n">
+        <v>652185</v>
+      </c>
+      <c r="D5" t="n">
+        <v>6.029866933822632</v>
+      </c>
+      <c r="E5" t="n">
+        <v>6.884910066784119</v>
+      </c>
+      <c r="F5" t="n">
+        <v>9</v>
+      </c>
+      <c r="G5" t="n">
+        <v>234</v>
+      </c>
+      <c r="H5" t="n">
+        <v>127</v>
+      </c>
+      <c r="I5" t="inlineStr"/>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
           <t>Future</t>
         </is>
       </c>
-      <c r="B4" t="inlineStr">
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Exact</t>
+        </is>
+      </c>
+      <c r="C6" t="n">
+        <v>508000</v>
+      </c>
+      <c r="D6" t="n">
+        <v>0.2557501792907715</v>
+      </c>
+      <c r="E6" t="n">
+        <v>0</v>
+      </c>
+      <c r="F6" t="n">
+        <v>3</v>
+      </c>
+      <c r="G6" t="n">
+        <v>256</v>
+      </c>
+      <c r="H6" t="n">
+        <v>98</v>
+      </c>
+      <c r="I6" t="inlineStr"/>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Future</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
         <is>
           <t>Heuristic</t>
         </is>
       </c>
-      <c r="C4" t="n">
+      <c r="C7" t="n">
         <v>537820</v>
       </c>
-      <c r="D4" t="n">
-        <v>6.489912748336792</v>
-      </c>
-      <c r="E4" t="inlineStr"/>
-      <c r="F4" t="n">
+      <c r="D7" t="n">
+        <v>6.508527994155884</v>
+      </c>
+      <c r="E7" t="n">
+        <v>5.870078740157481</v>
+      </c>
+      <c r="F7" t="n">
         <v>8</v>
       </c>
-      <c r="G4" t="n">
+      <c r="G7" t="n">
         <v>261</v>
       </c>
-      <c r="H4" t="n">
+      <c r="H7" t="n">
         <v>99</v>
       </c>
-      <c r="I4" t="inlineStr"/>
+      <c r="I7" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>